<commit_message>
Common: RTK info in FrSky Passthrough
</commit_message>
<xml_diff>
--- a/images/FrSky_Passthrough_protocol.xlsx
+++ b/images/FrSky_Passthrough_protocol.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\My Documents\Desktop\Dropbox\Craft and Theory\Products\FlightDeck\Promo\wiki\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\arduwiki\arduwiki2\ardupilot_wiki\images\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="7335" windowHeight="9420"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="7338" windowHeight="9420"/>
   </bookViews>
   <sheets>
     <sheet name="Passthrough" sheetId="9" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="69">
   <si>
     <t>Bits</t>
   </si>
@@ -116,9 +116,6 @@
     <t>Vertical velocity</t>
   </si>
   <si>
-    <t>Vertical dilution of precision</t>
-  </si>
-  <si>
     <t>decimeters/s</t>
   </si>
   <si>
@@ -225,12 +222,21 @@
   </si>
   <si>
     <t>Angle from front of vehicle to the direction of home</t>
+  </si>
+  <si>
+    <t>GPS advanced fix</t>
+  </si>
+  <si>
+    <t>0: no advanced fix, 1: DGPS, 2: RTK_FLOAT, 3: RTK_FIXED</t>
+  </si>
+  <si>
+    <t>RESERVED</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0000"/>
   </numFmts>
@@ -361,21 +367,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -395,6 +386,21 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -678,93 +684,93 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E37" sqref="E37"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="7.28515625" style="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="48.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.140625" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="60.28515625" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="7"/>
+    <col min="1" max="1" width="7.26171875" style="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="48.26171875" style="7" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.15625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.26171875" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="60.26171875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="9.15625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="25" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+    <row r="1" spans="1:5" s="20" customFormat="1" ht="14.7" thickBot="1" x14ac:dyDescent="0.6">
+      <c r="A1" s="21" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="22">
+        <v>800</v>
+      </c>
+      <c r="B2" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="B1" s="25" t="s">
-        <v>2</v>
-      </c>
-      <c r="C1" s="25" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="25" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" s="18" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="27">
-        <v>800</v>
-      </c>
-      <c r="B2" s="18" t="s">
-        <v>53</v>
-      </c>
       <c r="E2" s="18" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="28"/>
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="23"/>
       <c r="B3" s="3" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D3" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="28"/>
+    <row r="4" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="23"/>
       <c r="B4" s="3" t="s">
         <v>24</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D4" s="3">
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="29"/>
-    </row>
-    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="30">
+    <row r="5" spans="1:5" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="24"/>
+    </row>
+    <row r="6" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="25">
         <v>5000</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D6" s="8">
         <v>32</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B7" s="36" t="s">
-        <v>62</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+      <c r="B7" s="31" t="s">
+        <v>61</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>7</v>
@@ -773,12 +779,12 @@
         <v>3</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B8" s="19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>7</v>
@@ -788,18 +794,18 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="28"/>
-    </row>
-    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="30">
+    <row r="9" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="23"/>
+    </row>
+    <row r="10" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="25">
         <v>5001</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B11" s="7" t="s">
         <v>8</v>
       </c>
@@ -810,7 +816,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B12" s="7" t="s">
         <v>9</v>
       </c>
@@ -821,7 +827,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B13" s="7" t="s">
         <v>11</v>
       </c>
@@ -832,7 +838,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B14" s="7" t="s">
         <v>10</v>
       </c>
@@ -843,7 +849,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="B15" s="7" t="s">
         <v>17</v>
       </c>
@@ -854,10 +860,10 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="28"/>
+    <row r="16" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="23"/>
       <c r="B16" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>7</v>
@@ -867,32 +873,32 @@
       </c>
       <c r="E16" s="12"/>
     </row>
-    <row r="17" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="31"/>
-    </row>
-    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="30">
+    <row r="17" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="26"/>
+    </row>
+    <row r="18" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="25">
         <v>5002</v>
       </c>
       <c r="B18" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B19" s="7" t="s">
         <v>4</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D19" s="7">
         <v>4</v>
       </c>
       <c r="E19" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B20" s="7" t="s">
         <v>5</v>
       </c>
@@ -906,20 +912,20 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="20" t="s">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B21" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D21" s="4">
         <v>1</v>
       </c>
       <c r="E21" s="17"/>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="20"/>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B22" s="36"/>
       <c r="C22" s="4" t="s">
         <v>28</v>
       </c>
@@ -928,46 +934,46 @@
       </c>
       <c r="F22" s="17"/>
     </row>
-    <row r="23" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="28"/>
-      <c r="B23" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="4">
-        <v>1</v>
-      </c>
-      <c r="E23" s="4"/>
-    </row>
-    <row r="24" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="28"/>
-      <c r="B24" s="20"/>
-      <c r="C24" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="4">
-        <v>7</v>
-      </c>
-      <c r="E24" s="4"/>
-    </row>
-    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="28"/>
-      <c r="B25" s="22" t="s">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="7"/>
+      <c r="B23" s="7" t="s">
+        <v>66</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D23" s="7">
+        <v>2</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="7"/>
+      <c r="B24" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D24" s="7">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="23"/>
+      <c r="B25" s="35" t="s">
         <v>25</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D25" s="4">
         <v>2</v>
       </c>
       <c r="E25" s="17"/>
     </row>
-    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="28"/>
-      <c r="B26" s="22"/>
+    <row r="26" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A26" s="23"/>
+      <c r="B26" s="35"/>
       <c r="C26" s="4" t="s">
         <v>28</v>
       </c>
@@ -976,94 +982,94 @@
       </c>
       <c r="E26" s="17"/>
     </row>
-    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="22"/>
+    <row r="27" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="23"/>
+      <c r="B27" s="35"/>
       <c r="C27" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="7">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="30">
+    <row r="29" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A29" s="25">
         <v>5003</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B30" s="7" t="s">
         <v>3</v>
       </c>
       <c r="C30" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="7">
         <v>9</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B31" s="21" t="s">
-        <v>44</v>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B31" s="32" t="s">
+        <v>43</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D31" s="4">
         <v>1</v>
       </c>
       <c r="E31" s="17"/>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B32" s="21"/>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B32" s="32"/>
       <c r="C32" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D32" s="4">
         <v>7</v>
       </c>
       <c r="E32" s="17"/>
     </row>
-    <row r="33" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="32"/>
+    <row r="33" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A33" s="27"/>
       <c r="B33" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D33" s="3">
         <v>15</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="30">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A35" s="25">
         <v>5004</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B36" s="23" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B36" s="33" t="s">
         <v>12</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D36" s="7">
         <v>2</v>
       </c>
       <c r="E36" s="17"/>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B37" s="21"/>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B37" s="32"/>
       <c r="C37" s="7" t="s">
         <v>14</v>
       </c>
@@ -1072,9 +1078,9 @@
       </c>
       <c r="F37" s="17"/>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B38" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>13</v>
@@ -1084,20 +1090,20 @@
       </c>
       <c r="E38" s="17"/>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B39" s="21" t="s">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B39" s="32" t="s">
         <v>16</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D39" s="7">
         <v>2</v>
       </c>
       <c r="E39" s="17"/>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B40" s="21"/>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B40" s="32"/>
       <c r="C40" s="7" t="s">
         <v>28</v>
       </c>
@@ -1106,82 +1112,82 @@
       </c>
       <c r="F40" s="17"/>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="21"/>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B41" s="32"/>
       <c r="C41" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D41" s="7">
         <v>1</v>
       </c>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="35"/>
-    </row>
-    <row r="43" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="30">
+    <row r="42" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A42" s="30"/>
+    </row>
+    <row r="43" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A43" s="25">
         <v>5005</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="31"/>
-      <c r="B44" s="23" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A44" s="26"/>
+      <c r="B44" s="33" t="s">
         <v>29</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D44" s="11">
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B45" s="24"/>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B45" s="34"/>
       <c r="C45" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D45" s="7">
         <v>7</v>
       </c>
       <c r="E45" s="17"/>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B46" s="24"/>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B46" s="34"/>
       <c r="C46" s="16" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46" s="7">
         <v>1</v>
       </c>
       <c r="E46" s="6"/>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B47" s="21" t="s">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B47" s="32" t="s">
         <v>18</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D47" s="7">
         <v>1</v>
       </c>
       <c r="E47" s="17"/>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B48" s="21"/>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B48" s="32"/>
       <c r="C48" s="7" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D48" s="7">
         <v>7</v>
       </c>
       <c r="F48" s="17"/>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B49" s="7" t="s">
         <v>21</v>
       </c>
@@ -1192,19 +1198,19 @@
         <v>11</v>
       </c>
     </row>
-    <row r="50" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="32"/>
+    <row r="50" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A50" s="27"/>
       <c r="B50" s="10"/>
     </row>
-    <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="30">
+    <row r="51" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A51" s="25">
         <v>5006</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B52" s="7" t="s">
         <v>19</v>
       </c>
@@ -1216,7 +1222,7 @@
       </c>
       <c r="E52" s="16"/>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B53" s="7" t="s">
         <v>20</v>
       </c>
@@ -1228,20 +1234,20 @@
       </c>
       <c r="E53" s="16"/>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B54" s="21" t="s">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B54" s="32" t="s">
         <v>26</v>
       </c>
       <c r="C54" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D54" s="7">
         <v>1</v>
       </c>
       <c r="E54" s="17"/>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B55" s="21"/>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.55000000000000004">
+      <c r="B55" s="32"/>
       <c r="C55" s="7" t="s">
         <v>15</v>
       </c>
@@ -1250,16 +1256,16 @@
       </c>
       <c r="F55" s="17"/>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.55000000000000004">
       <c r="B56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="30">
+    <row r="57" spans="1:6" s="8" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A57" s="25">
         <v>5007</v>
       </c>
       <c r="B57" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C57" s="14" t="s">
         <v>7</v>
@@ -1268,13 +1274,13 @@
         <v>8</v>
       </c>
       <c r="E57" s="8" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="31"/>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" s="11" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A58" s="26"/>
       <c r="B58" s="9" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>7</v>
@@ -1283,39 +1289,39 @@
         <v>8</v>
       </c>
     </row>
-    <row r="59" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="32"/>
+    <row r="59" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A59" s="27"/>
       <c r="B59" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D59" s="3">
         <v>24</v>
       </c>
       <c r="E59" s="11"/>
     </row>
-    <row r="60" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="32"/>
+    <row r="60" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A60" s="27"/>
       <c r="B60" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D60" s="3">
         <v>24</v>
       </c>
       <c r="E60" s="11"/>
     </row>
-    <row r="61" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="33"/>
+    <row r="61" spans="1:6" s="13" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A61" s="28"/>
       <c r="B61" s="9" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C61" s="11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D61" s="9">
         <v>24</v>
@@ -1323,16 +1329,15 @@
       <c r="E61" s="15"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
+  <mergeCells count="8">
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="B31:B32"/>
     <mergeCell ref="B47:B48"/>
     <mergeCell ref="B54:B55"/>
     <mergeCell ref="B39:B41"/>
     <mergeCell ref="B44:B46"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="B36:B37"/>
-    <mergeCell ref="B21:B22"/>
-    <mergeCell ref="B23:B24"/>
-    <mergeCell ref="B31:B32"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>